<commit_message>
3280 convert date to binary
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tampere University\Ms in CSE\Year 2024-2025\1. Autumn\2-1\project-self\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99C3407-A64C-4A7D-8970-1C7881179753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD0484-953B-4551-8053-621C6BF51FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +92,14 @@
       <u/>
       <sz val="14"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +174,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -451,7 +462,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -483,11 +494,11 @@
     <row r="2" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45536</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">

</xml_diff>